<commit_message>
Changes for VAR model and duplicate data removal
</commit_message>
<xml_diff>
--- a/Frequency_Of_Words.xlsx
+++ b/Frequency_Of_Words.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4394</v>
+        <v>653</v>
       </c>
       <c r="D2" t="n">
         <v>1</v>
@@ -480,11 +480,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>deaths</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3661</v>
+        <v>638</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
@@ -499,11 +499,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>reported</t>
+          <t>incidence</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3336</v>
+        <v>605</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -518,11 +518,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>today</t>
+          <t>new infections</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3218</v>
+        <v>605</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -537,11 +537,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>7 day average</t>
+          <t>infected</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3126</v>
+        <v>410</v>
       </c>
       <c r="D6" t="n">
         <v>1</v>
@@ -556,11 +556,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>white</t>
+          <t>people</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>2022</v>
+        <v>401</v>
       </c>
       <c r="D7" t="n">
         <v>1</v>
@@ -575,11 +575,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>protect</t>
+          <t>persons</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1670</v>
+        <v>347</v>
       </c>
       <c r="D8" t="n">
         <v>1</v>
@@ -594,11 +594,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>deaths</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1635</v>
+        <v>320</v>
       </c>
       <c r="D9" t="n">
         <v>1</v>
@@ -613,11 +613,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>mutants</t>
+          <t>pandemic</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1623</v>
+        <v>319</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
@@ -632,11 +632,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>new infections</t>
+          <t>compulsory vaccination</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1388</v>
+        <v>285</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
@@ -651,11 +651,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2795</v>
+        <v>455</v>
       </c>
       <c r="D12" t="n">
         <v>2</v>
@@ -670,11 +670,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>deaths</t>
+          <t>incidence</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2320</v>
+        <v>454</v>
       </c>
       <c r="D13" t="n">
         <v>2</v>
@@ -689,11 +689,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>reported</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2015</v>
+        <v>412</v>
       </c>
       <c r="D14" t="n">
         <v>2</v>
@@ -708,11 +708,11 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>today</t>
+          <t>new infections</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1949</v>
+        <v>382</v>
       </c>
       <c r="D15" t="n">
         <v>2</v>
@@ -727,11 +727,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>speaks</t>
+          <t>people</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1944</v>
+        <v>306</v>
       </c>
       <c r="D16" t="n">
         <v>2</v>
@@ -746,11 +746,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>laboratory</t>
+          <t>infected</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1942</v>
+        <v>304</v>
       </c>
       <c r="D17" t="n">
         <v>2</v>
@@ -765,11 +765,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>developed</t>
+          <t>deaths</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1917</v>
+        <v>268</v>
       </c>
       <c r="D18" t="n">
         <v>2</v>
@@ -784,11 +784,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>American</t>
+          <t>persons</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1912</v>
+        <v>256</v>
       </c>
       <c r="D19" t="n">
         <v>2</v>
@@ -803,11 +803,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>emails</t>
+          <t>pandemic</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1911</v>
+        <v>215</v>
       </c>
       <c r="D20" t="n">
         <v>2</v>
@@ -822,11 +822,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>chief immunologist</t>
+          <t>gives</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>1910</v>
+        <v>208</v>
       </c>
       <c r="D21" t="n">
         <v>2</v>
@@ -841,11 +841,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>incidence</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1314</v>
+        <v>449</v>
       </c>
       <c r="D22" t="n">
         <v>3</v>
@@ -860,11 +860,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>incidence</t>
+          <t>new infections</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1273</v>
+        <v>413</v>
       </c>
       <c r="D23" t="n">
         <v>3</v>
@@ -879,11 +879,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>deaths</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1139</v>
+        <v>371</v>
       </c>
       <c r="D24" t="n">
         <v>3</v>
@@ -898,11 +898,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>masks</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1124</v>
+        <v>335</v>
       </c>
       <c r="D25" t="n">
         <v>3</v>
@@ -921,7 +921,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1004</v>
+        <v>309</v>
       </c>
       <c r="D26" t="n">
         <v>3</v>
@@ -936,11 +936,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>traffic light coalition</t>
+          <t>persons</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>951</v>
+        <v>285</v>
       </c>
       <c r="D27" t="n">
         <v>3</v>
@@ -955,11 +955,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>company</t>
+          <t>pandemic</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>932</v>
+        <v>279</v>
       </c>
       <c r="D28" t="n">
         <v>3</v>
@@ -974,11 +974,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>reported</t>
+          <t>infected</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>921</v>
+        <v>232</v>
       </c>
       <c r="D29" t="n">
         <v>3</v>
@@ -993,11 +993,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>decided</t>
+          <t>deaths</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>921</v>
+        <v>229</v>
       </c>
       <c r="D30" t="n">
         <v>3</v>
@@ -1012,11 +1012,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>contracts</t>
+          <t>gives</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>909</v>
+        <v>228</v>
       </c>
       <c r="D31" t="n">
         <v>3</v>
@@ -1031,11 +1031,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>variants</t>
+          <t>incidence</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>1208</v>
+        <v>284</v>
       </c>
       <c r="D32" t="n">
         <v>4</v>
@@ -1050,11 +1050,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1116</v>
+        <v>254</v>
       </c>
       <c r="D33" t="n">
         <v>4</v>
@@ -1069,11 +1069,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>killer variants</t>
+          <t>new infections</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>1105</v>
+        <v>237</v>
       </c>
       <c r="D34" t="n">
         <v>4</v>
@@ -1088,11 +1088,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>vaccination</t>
+          <t>people</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>766</v>
+        <v>195</v>
       </c>
       <c r="D35" t="n">
         <v>4</v>
@@ -1107,11 +1107,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>incidence</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>488</v>
+        <v>184</v>
       </c>
       <c r="D36" t="n">
         <v>4</v>
@@ -1126,11 +1126,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>compulsory vaccination</t>
+          <t>data</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>453</v>
+        <v>166</v>
       </c>
       <c r="D37" t="n">
         <v>4</v>
@@ -1145,11 +1145,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>infections</t>
+          <t>persons</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>449</v>
+        <v>156</v>
       </c>
       <c r="D38" t="n">
         <v>4</v>
@@ -1164,11 +1164,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>new infections</t>
+          <t>deaths</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>425</v>
+        <v>155</v>
       </c>
       <c r="D39" t="n">
         <v>4</v>
@@ -1183,11 +1183,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>more</t>
+          <t>infections</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>425</v>
+        <v>151</v>
       </c>
       <c r="D40" t="n">
         <v>4</v>
@@ -1202,11 +1202,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>people</t>
+          <t>pandemic</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>420</v>
+        <v>139</v>
       </c>
       <c r="D41" t="n">
         <v>4</v>
@@ -1221,11 +1221,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>autumn</t>
+          <t>new infections</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>724</v>
+        <v>214</v>
       </c>
       <c r="D42" t="n">
         <v>5</v>
@@ -1240,11 +1240,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>months</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>691</v>
+        <v>201</v>
       </c>
       <c r="D43" t="n">
         <v>5</v>
@@ -1259,11 +1259,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>development</t>
+          <t>incidence</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>653</v>
+        <v>180</v>
       </c>
       <c r="D44" t="n">
         <v>5</v>
@@ -1278,11 +1278,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>pandemic</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>623</v>
+        <v>176</v>
       </c>
       <c r="D45" t="n">
         <v>5</v>
@@ -1297,11 +1297,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>years</t>
+          <t>people</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>608</v>
+        <v>176</v>
       </c>
       <c r="D46" t="n">
         <v>5</v>
@@ -1316,11 +1316,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>schoolchildren</t>
+          <t>monkeypox</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>594</v>
+        <v>158</v>
       </c>
       <c r="D47" t="n">
         <v>5</v>
@@ -1335,11 +1335,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>pointed out</t>
+          <t>deaths</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>594</v>
+        <v>133</v>
       </c>
       <c r="D48" t="n">
         <v>5</v>
@@ -1354,11 +1354,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>dramatic</t>
+          <t>infections</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>594</v>
+        <v>119</v>
       </c>
       <c r="D49" t="n">
         <v>5</v>
@@ -1373,11 +1373,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>politics</t>
+          <t>pandemic</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>507</v>
+        <v>115</v>
       </c>
       <c r="D50" t="n">
         <v>5</v>
@@ -1392,11 +1392,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>give</t>
+          <t>data</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>484</v>
+        <v>110</v>
       </c>
       <c r="D51" t="n">
         <v>5</v>
@@ -1411,11 +1411,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>last</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1090</v>
+        <v>212</v>
       </c>
       <c r="D52" t="n">
         <v>6</v>
@@ -1430,11 +1430,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>data</t>
+          <t>new infections</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1064</v>
+        <v>180</v>
       </c>
       <c r="D53" t="n">
         <v>6</v>
@@ -1449,11 +1449,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>wave</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>1005</v>
+        <v>156</v>
       </c>
       <c r="D54" t="n">
         <v>6</v>
@@ -1468,11 +1468,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>large part</t>
+          <t>people</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>964</v>
+        <v>150</v>
       </c>
       <c r="D55" t="n">
         <v>6</v>
@@ -1487,11 +1487,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>deceased</t>
+          <t>incidence</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>955</v>
+        <v>145</v>
       </c>
       <c r="D56" t="n">
         <v>6</v>
@@ -1506,11 +1506,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>impressive</t>
+          <t>gives</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>949</v>
+        <v>135</v>
       </c>
       <c r="D57" t="n">
         <v>6</v>
@@ -1525,11 +1525,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>gives</t>
+          <t>autumn</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>896</v>
+        <v>114</v>
       </c>
       <c r="D58" t="n">
         <v>6</v>
@@ -1544,11 +1544,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>people</t>
+          <t>children</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>873</v>
+        <v>113</v>
       </c>
       <c r="D59" t="n">
         <v>6</v>
@@ -1563,11 +1563,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>pandemic</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>747</v>
+        <v>100</v>
       </c>
       <c r="D60" t="n">
         <v>6</v>
@@ -1582,11 +1582,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>children</t>
+          <t>pay</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>674</v>
+        <v>93</v>
       </c>
       <c r="D61" t="n">
         <v>6</v>
@@ -1601,11 +1601,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>current</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1198</v>
+        <v>228</v>
       </c>
       <c r="D62" t="n">
         <v>7</v>
@@ -1620,11 +1620,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>chaos</t>
+          <t>new infections</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>1020</v>
+        <v>163</v>
       </c>
       <c r="D63" t="n">
         <v>7</v>
@@ -1639,11 +1639,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>economic</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>997</v>
+        <v>141</v>
       </c>
       <c r="D64" t="n">
         <v>7</v>
@@ -1658,11 +1658,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>social</t>
+          <t>people</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>997</v>
+        <v>140</v>
       </c>
       <c r="D65" t="n">
         <v>7</v>
@@ -1677,11 +1677,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>masks</t>
+          <t>incidence</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>984</v>
+        <v>119</v>
       </c>
       <c r="D66" t="n">
         <v>7</v>
@@ -1696,11 +1696,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>data</t>
+          <t>gives</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>869</v>
+        <v>112</v>
       </c>
       <c r="D67" t="n">
         <v>7</v>
@@ -1715,11 +1715,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>immune system</t>
+          <t>infection</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>704</v>
+        <v>94</v>
       </c>
       <c r="D68" t="n">
         <v>7</v>
@@ -1734,11 +1734,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>carry</t>
+          <t>pandemic</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>645</v>
+        <v>90</v>
       </c>
       <c r="D69" t="n">
         <v>7</v>
@@ -1753,11 +1753,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>people</t>
+          <t>7-day #incidence</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>632</v>
+        <v>87</v>
       </c>
       <c r="D70" t="n">
         <v>7</v>
@@ -1772,11 +1772,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>recommendation</t>
+          <t>infected</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>603</v>
+        <v>82</v>
       </c>
       <c r="D71" t="n">
         <v>7</v>
@@ -1791,11 +1791,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>measures</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>1148</v>
+        <v>176</v>
       </c>
       <c r="D72" t="n">
         <v>8</v>
@@ -1810,11 +1810,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>circulates</t>
+          <t>new infections</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>1090</v>
+        <v>140</v>
       </c>
       <c r="D73" t="n">
         <v>8</v>
@@ -1829,11 +1829,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>worked</t>
+          <t>infection</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>1089</v>
+        <v>115</v>
       </c>
       <c r="D74" t="n">
         <v>8</v>
@@ -1848,11 +1848,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>analysis</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>994</v>
+        <v>114</v>
       </c>
       <c r="D75" t="n">
         <v>8</v>
@@ -1867,11 +1867,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>scientist</t>
+          <t>incidence</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>989</v>
+        <v>106</v>
       </c>
       <c r="D76" t="n">
         <v>8</v>
@@ -1886,11 +1886,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>worth reading</t>
+          <t>gives</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>977</v>
+        <v>94</v>
       </c>
       <c r="D77" t="n">
         <v>8</v>
@@ -1905,11 +1905,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>recognized</t>
+          <t>7-day #incidence</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>977</v>
+        <v>94</v>
       </c>
       <c r="D78" t="n">
         <v>8</v>
@@ -1924,11 +1924,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>study</t>
+          <t>people</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>976</v>
+        <v>92</v>
       </c>
       <c r="D79" t="n">
         <v>8</v>
@@ -1943,11 +1943,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>have</t>
+          <t>deaths</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>887</v>
+        <v>73</v>
       </c>
       <c r="D80" t="n">
         <v>8</v>
@@ -1962,11 +1962,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>life</t>
+          <t>study</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>855</v>
+        <v>71</v>
       </c>
       <c r="D81" t="n">
         <v>8</v>
@@ -1981,11 +1981,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>infection</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1697</v>
+        <v>153</v>
       </c>
       <c r="D82" t="n">
         <v>9</v>
@@ -2000,11 +2000,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>flu</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>904</v>
+        <v>107</v>
       </c>
       <c r="D83" t="n">
         <v>9</v>
@@ -2019,11 +2019,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>lies</t>
+          <t>new infections</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>834</v>
+        <v>95</v>
       </c>
       <c r="D84" t="n">
         <v>9</v>
@@ -2038,11 +2038,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>case mortality</t>
+          <t>incidence</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>820</v>
+        <v>87</v>
       </c>
       <c r="D85" t="n">
         <v>9</v>
@@ -2057,11 +2057,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>trains</t>
+          <t>pandemic</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>765</v>
+        <v>79</v>
       </c>
       <c r="D86" t="n">
         <v>9</v>
@@ -2076,11 +2076,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>vaccination</t>
+          <t>gives</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>579</v>
+        <v>77</v>
       </c>
       <c r="D87" t="n">
         <v>9</v>
@@ -2095,11 +2095,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Mr</t>
+          <t>7-day #incidence</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>461</v>
+        <v>76</v>
       </c>
       <c r="D88" t="n">
         <v>9</v>
@@ -2114,11 +2114,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>buses</t>
+          <t>people</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>444</v>
+        <v>67</v>
       </c>
       <c r="D89" t="n">
         <v>9</v>
@@ -2133,11 +2133,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>feels</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>442</v>
+        <v>63</v>
       </c>
       <c r="D90" t="n">
         <v>9</v>
@@ -2152,11 +2152,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>ffp2-#mask requirement</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>442</v>
+        <v>62</v>
       </c>
       <c r="D91" t="n">
         <v>9</v>
@@ -2171,11 +2171,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>infection</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>797</v>
+        <v>182</v>
       </c>
       <c r="D92" t="n">
         <v>10</v>
@@ -2190,11 +2190,11 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>vaccination</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>769</v>
+        <v>132</v>
       </c>
       <c r="D93" t="n">
         <v>10</v>
@@ -2209,11 +2209,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>months</t>
+          <t>new infections</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>595</v>
+        <v>129</v>
       </c>
       <c r="D94" t="n">
         <v>10</v>
@@ -2228,11 +2228,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>cause</t>
+          <t>people</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>592</v>
+        <v>107</v>
       </c>
       <c r="D95" t="n">
         <v>10</v>
@@ -2247,11 +2247,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>long term</t>
+          <t>incidence</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>588</v>
+        <v>97</v>
       </c>
       <c r="D96" t="n">
         <v>10</v>
@@ -2266,11 +2266,11 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>heart damage</t>
+          <t>7-day #incidence</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>586</v>
+        <v>79</v>
       </c>
       <c r="D97" t="n">
         <v>10</v>
@@ -2285,11 +2285,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>research results</t>
+          <t>pandemic</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>586</v>
+        <v>73</v>
       </c>
       <c r="D98" t="n">
         <v>10</v>
@@ -2304,11 +2304,11 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>mask</t>
+          <t>gives</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>557</v>
+        <v>72</v>
       </c>
       <c r="D99" t="n">
         <v>10</v>
@@ -2327,7 +2327,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>533</v>
+        <v>71</v>
       </c>
       <c r="D100" t="n">
         <v>10</v>
@@ -2346,7 +2346,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>529</v>
+        <v>66</v>
       </c>
       <c r="D101" t="n">
         <v>10</v>
@@ -2361,11 +2361,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>pandemic</t>
+          <t>vaccination</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>910</v>
+        <v>74</v>
       </c>
       <c r="D102" t="n">
         <v>11</v>
@@ -2380,11 +2380,11 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>start</t>
+          <t>children</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>884</v>
+        <v>51</v>
       </c>
       <c r="D103" t="n">
         <v>11</v>
@@ -2399,11 +2399,11 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>years</t>
+          <t>people</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>875</v>
+        <v>49</v>
       </c>
       <c r="D104" t="n">
         <v>11</v>
@@ -2418,11 +2418,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>expectations</t>
+          <t>new infections</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>867</v>
+        <v>47</v>
       </c>
       <c r="D105" t="n">
         <v>11</v>
@@ -2437,11 +2437,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>behavioral</t>
+          <t>incidence</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>867</v>
+        <v>35</v>
       </c>
       <c r="D106" t="n">
         <v>11</v>
@@ -2456,11 +2456,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>initial</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>867</v>
+        <v>34</v>
       </c>
       <c r="D107" t="n">
         <v>11</v>
@@ -2475,11 +2475,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>coming</t>
+          <t>study</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>812</v>
+        <v>33</v>
       </c>
       <c r="D108" t="n">
         <v>11</v>
@@ -2494,11 +2494,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>unvaccinated</t>
+          <t>new</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>796</v>
+        <v>32</v>
       </c>
       <c r="D109" t="n">
         <v>11</v>
@@ -2513,11 +2513,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>rush</t>
+          <t>infection</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>793</v>
+        <v>29</v>
       </c>
       <c r="D110" t="n">
         <v>11</v>
@@ -2532,11 +2532,11 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>hate</t>
+          <t>7-day #incidence</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>792</v>
+        <v>25</v>
       </c>
       <c r="D111" t="n">
         <v>11</v>

</xml_diff>